<commit_message>
Enforce HH ID/ExtID format
</commit_message>
<xml_diff>
--- a/odkx/forms/hh_member_absent.xlsx
+++ b/odkx/forms/hh_member_absent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="505">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1190,6 +1190,9 @@
     <t xml:space="preserve">valuesList</t>
   </si>
   <si>
+    <t xml:space="preserve">isSessionVariable</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assigned by household form</t>
   </si>
   <si>
@@ -1203,6 +1206,9 @@
   </si>
   <si>
     <t xml:space="preserve">hh_head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_candidate</t>
   </si>
   <si>
     <t xml:space="preserve">Registration</t>
@@ -1819,7 +1825,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.7"/>
   </cols>
@@ -2864,7 +2870,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
@@ -4267,7 +4273,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -7095,18 +7101,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7122,491 +7129,494 @@
       <c r="D1" s="0" t="s">
         <v>387</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>391</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
-        <v>395</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>396</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="6" t="s">
-        <v>189</v>
+        <v>405</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>189</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
-        <v>326</v>
+        <v>189</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>326</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
-        <v>404</v>
+        <v>326</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>394</v>
+        <v>16</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D19" s="0" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="B24" s="8" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="C31" s="9" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D32" s="0" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="9" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>46</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D38" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>421</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="C38" s="6" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D39" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="C39" s="6" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D40" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="C40" s="10" t="s">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="10" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>46</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="10" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="10" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="10" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>394</v>
+        <v>29</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="10" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C47" s="10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D48" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>434</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>435</v>
+      </c>
       <c r="B49" s="11" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>16</v>
@@ -7617,7 +7627,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>16</v>
@@ -7628,10 +7638,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="11" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>438</v>
+        <v>16</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7639,261 +7652,258 @@
         <v>439</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>41</v>
+        <v>440</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="11" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>438</v>
+        <v>16</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="11" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="11" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>290</v>
+        <v>440</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="11" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="11" t="s">
-        <v>199</v>
+        <v>445</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>199</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="11" t="s">
-        <v>444</v>
+        <v>199</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>445</v>
+        <v>16</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>446</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="D59" s="0" t="s">
-        <v>361</v>
+        <v>448</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="11" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>126</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="11" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>394</v>
+        <v>29</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="11" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>46</v>
+        <v>396</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="11" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>273</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="11" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>394</v>
+        <v>29</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="11" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>279</v>
+        <v>396</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="11" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>394</v>
+        <v>29</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="11" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>41</v>
+        <v>396</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="11" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>172</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="11" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>394</v>
+        <v>29</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="11" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>46</v>
+        <v>396</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="11" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>233</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="11" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>46</v>
+        <v>233</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="11" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>228</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="11" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="11" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>47</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="11" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>16</v>
@@ -7904,7 +7914,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="11" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>16</v>
@@ -7915,182 +7925,193 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="11" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>221</v>
+        <v>47</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="11" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>121</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="11" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="11" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>211</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="11" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="11" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="11" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="11" t="s">
-        <v>346</v>
+        <v>475</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>346</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="11" t="s">
-        <v>474</v>
+        <v>346</v>
       </c>
       <c r="C87" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="11" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>76</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="11" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>335</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="11" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C90" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="11" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>94</v>
+        <v>347</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="11" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="11" t="s">
-        <v>348</v>
+        <v>481</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>348</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="11" t="s">
-        <v>480</v>
+        <v>348</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>50</v>
+        <v>348</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="11" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C95" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="C96" s="11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -8112,16 +8133,16 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="21.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="21.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="8.7"/>
@@ -8129,41 +8150,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20210124001</v>
@@ -8171,29 +8192,29 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -8201,44 +8222,44 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>